<commit_message>
Tooltips added and improved for all charts
</commit_message>
<xml_diff>
--- a/data-viz/inputs/region_labels.xlsx
+++ b/data-viz/inputs/region_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-thematic-reports/data-viz/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA9D4AB-FCD9-484E-A0B9-05B688B02FDF}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B5ABD2E-53D4-4CE8-AF34-B8B6A6AE4A85}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2324,7 +2324,7 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2333,7 @@
     <col min="2" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="48.28515625" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
@@ -6341,12 +6341,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6599,20 +6601,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C746D7-CF54-4E7D-92A4-AB36B233844F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6637,12 +6640,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C746D7-CF54-4E7D-92A4-AB36B233844F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Secound round of final charts
</commit_message>
<xml_diff>
--- a/data-viz/inputs/region_labels.xlsx
+++ b/data-viz/inputs/region_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-thematic-reports/data-viz/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B5ABD2E-53D4-4CE8-AF34-B8B6A6AE4A85}"/>
+  <xr:revisionPtr revIDLastSave="402" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A1067F7-EEFD-4505-93F0-6758009D6EB2}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2324,20 +2324,20 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="15"/>
+    <col min="2" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>324</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>155</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>182</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>17</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>300</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>300</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>300</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>300</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>89</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>89</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>197</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>197</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>169</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>185</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>188</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>188</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>195</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>207</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>209</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>209</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>209</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>209</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>232</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>232</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>232</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>232</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>232</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>232</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>254</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>254</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>254</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>266</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>266</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>266</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>266</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>286</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>286</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>286</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>286</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>279</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>279</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>102</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>309</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>309</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>309</v>
       </c>
@@ -6341,17 +6341,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3620e9c0d1a16779aea146adda0186f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2afd3ea0446edf26a13b3c7fc9e6232" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -6600,6 +6589,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6610,17 +6610,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C746D7-CF54-4E7D-92A4-AB36B233844F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED2CE6EF-790B-4B69-B141-5B1187A2316D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6639,6 +6628,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C746D7-CF54-4E7D-92A4-AB36B233844F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed repeated variable in data4web
</commit_message>
<xml_diff>
--- a/data-viz/inputs/region_labels.xlsx
+++ b/data-viz/inputs/region_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-thematic-reports/data-viz/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A1067F7-EEFD-4505-93F0-6758009D6EB2}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069D605E-95FC-404C-9832-13E965666165}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2324,20 +2324,20 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="48.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="15"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>324</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>155</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>182</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>17</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>300</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>300</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>300</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>300</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>89</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>89</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>197</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>197</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>169</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>185</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>188</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>188</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>195</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>207</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>209</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>209</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>209</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>209</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>232</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>232</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>232</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>232</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>232</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>232</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>254</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>254</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>254</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>266</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>266</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>266</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>266</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>286</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>286</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>286</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>286</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>279</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>279</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>102</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>309</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>309</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>309</v>
       </c>
@@ -6590,6 +6590,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
@@ -6598,15 +6607,6 @@
     <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6629,6 +6629,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C746D7-CF54-4E7D-92A4-AB36B233844F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6637,12 +6645,4 @@
     <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Long names bug fixed in maps
</commit_message>
<xml_diff>
--- a/data-viz/inputs/region_labels.xlsx
+++ b/data-viz/inputs/region_labels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-thematic-reports/data-viz/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069D605E-95FC-404C-9832-13E965666165}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DFB7213-85B3-44B0-B4B2-F560E23478C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
   </bookViews>
@@ -1162,9 +1162,6 @@
     <t>Western and Central Bohemia</t>
   </si>
   <si>
-    <t>North-East and South- East</t>
-  </si>
-  <si>
     <t>Central Moravia and Silesia</t>
   </si>
   <si>
@@ -1853,6 +1850,9 @@
   </si>
   <si>
     <t>#19212B</t>
+  </si>
+  <si>
+    <t>North-East and South-East</t>
   </si>
 </sst>
 </file>
@@ -2324,7 +2324,7 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2333,7 @@
     <col min="2" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="48.28515625" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
@@ -2366,10 +2366,10 @@
         <v>362</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2402,10 +2402,10 @@
         <v>0.43951896873419782</v>
       </c>
       <c r="J2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2438,10 +2438,10 @@
         <v>0.20145282056486422</v>
       </c>
       <c r="J3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2474,10 +2474,10 @@
         <v>0.35902821070093793</v>
       </c>
       <c r="J4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2510,10 +2510,10 @@
         <v>0.10671887683308132</v>
       </c>
       <c r="J5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2546,10 +2546,10 @@
         <v>0.57805389789620798</v>
       </c>
       <c r="J6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2582,10 +2582,10 @@
         <v>0.31522722527071068</v>
       </c>
       <c r="J7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2618,10 +2618,10 @@
         <v>0.485463831344772</v>
       </c>
       <c r="J8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2654,10 +2654,10 @@
         <v>0.514536168655228</v>
       </c>
       <c r="J9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2690,10 +2690,10 @@
         <v>0.25944780614579366</v>
       </c>
       <c r="J10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2726,10 +2726,10 @@
         <v>0.33706121227953822</v>
       </c>
       <c r="J11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K11" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2762,10 +2762,10 @@
         <v>0.19959624959814526</v>
       </c>
       <c r="J12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2798,10 +2798,10 @@
         <v>0.20389473197652286</v>
       </c>
       <c r="J13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2834,10 +2834,10 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2870,10 +2870,10 @@
         <v>0.12535879608357547</v>
       </c>
       <c r="J15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>363</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>369</v>
@@ -2906,10 +2906,10 @@
         <v>0.35123563280227649</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2926,10 +2926,10 @@
         <v>364</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>370</v>
+        <v>600</v>
       </c>
       <c r="G17" s="16">
         <v>10827529</v>
@@ -2942,10 +2942,10 @@
         <v>0.30156298819425931</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2962,10 +2962,10 @@
         <v>368</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G18" s="16">
         <v>10827529</v>
@@ -2978,10 +2978,10 @@
         <v>0.22184258291988873</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3014,10 +3014,10 @@
         <v>0.31889117416926727</v>
       </c>
       <c r="J19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3050,10 +3050,10 @@
         <v>0.14325072724618695</v>
       </c>
       <c r="J20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3086,10 +3086,10 @@
         <v>0.20857663366176418</v>
       </c>
       <c r="J21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3122,10 +3122,10 @@
         <v>0.22905077558880055</v>
       </c>
       <c r="J22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K22" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3158,10 +3158,10 @@
         <v>0.10023068933398105</v>
       </c>
       <c r="J23" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3194,10 +3194,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3230,10 +3230,10 @@
         <v>0.24888002631214762</v>
       </c>
       <c r="J25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K25" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3266,10 +3266,10 @@
         <v>0.31147418120514669</v>
       </c>
       <c r="J26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K26" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3280,16 +3280,16 @@
         <v>2</v>
       </c>
       <c r="C27" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="E27" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>377</v>
-      </c>
       <c r="F27" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G27" s="16">
         <v>5563970</v>
@@ -3302,10 +3302,10 @@
         <v>0.21114995228227326</v>
       </c>
       <c r="J27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K27" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3338,10 +3338,10 @@
         <v>0.22849584020043243</v>
       </c>
       <c r="J28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3374,10 +3374,10 @@
         <v>0.18171992107664595</v>
       </c>
       <c r="J29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3410,10 +3410,10 @@
         <v>3.7738340222402196E-2</v>
       </c>
       <c r="J30" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3446,10 +3446,10 @@
         <v>4.0983511692616853E-2</v>
       </c>
       <c r="J31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K31" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3482,10 +3482,10 @@
         <v>4.8796094088717878E-2</v>
       </c>
       <c r="J32" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3518,10 +3518,10 @@
         <v>8.7812858751936271E-2</v>
       </c>
       <c r="J33" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K33" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3554,10 +3554,10 @@
         <v>8.1634721628776746E-2</v>
       </c>
       <c r="J34" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3590,10 +3590,10 @@
         <v>5.7238442146952159E-2</v>
       </c>
       <c r="J35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K35" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3626,10 +3626,10 @@
         <v>5.0355744329604379E-2</v>
       </c>
       <c r="J36" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K36" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3662,10 +3662,10 @@
         <v>8.9846289094871121E-2</v>
       </c>
       <c r="J37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3698,10 +3698,10 @@
         <v>8.9626407249312284E-2</v>
       </c>
       <c r="J38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K38" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3734,10 +3734,10 @@
         <v>0.12021687126850863</v>
       </c>
       <c r="J39" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K39" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3770,10 +3770,10 @@
         <v>7.5894470619934928E-2</v>
       </c>
       <c r="J40" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K40" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3806,10 +3806,10 @@
         <v>5.1758191519199756E-3</v>
       </c>
       <c r="J41" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K41" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3842,10 +3842,10 @@
         <v>0.13371753726595001</v>
       </c>
       <c r="J42" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K42" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3878,10 +3878,10 @@
         <v>0.15848240928381607</v>
       </c>
       <c r="J43" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K43" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3914,10 +3914,10 @@
         <v>4.4515201695803211E-2</v>
       </c>
       <c r="J44" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K44" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3950,10 +3950,10 @@
         <v>3.0502254979901635E-2</v>
       </c>
       <c r="J45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K45" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3986,10 +3986,10 @@
         <v>8.1184610813483746E-3</v>
       </c>
       <c r="J46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K46" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4022,10 +4022,10 @@
         <v>2.2429444120530575E-2</v>
       </c>
       <c r="J47" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K47" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4058,10 +4058,10 @@
         <v>7.5763958124367398E-2</v>
       </c>
       <c r="J48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K48" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -4094,10 +4094,10 @@
         <v>1.9302990694099711E-2</v>
       </c>
       <c r="J49" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K49" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4130,10 +4130,10 @@
         <v>9.6495417878231973E-2</v>
       </c>
       <c r="J50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -4166,10 +4166,10 @@
         <v>0.2150232853472567</v>
       </c>
       <c r="J51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K51" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -4202,10 +4202,10 @@
         <v>4.9303069524007828E-2</v>
       </c>
       <c r="J52" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -4238,10 +4238,10 @@
         <v>1.1767183393750828E-2</v>
       </c>
       <c r="J53" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K53" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -4274,10 +4274,10 @@
         <v>4.8437742361218908E-2</v>
       </c>
       <c r="J54" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K54" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -4310,10 +4310,10 @@
         <v>2.5920731845012816E-2</v>
       </c>
       <c r="J55" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K55" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -4346,10 +4346,10 @@
         <v>3.5008421464281549E-2</v>
       </c>
       <c r="J56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K56" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4382,10 +4382,10 @@
         <v>2.5211890940422432E-2</v>
       </c>
       <c r="J57" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K57" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4418,10 +4418,10 @@
         <v>0.36401464876739753</v>
       </c>
       <c r="J58" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K58" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4454,10 +4454,10 @@
         <v>0.10998319374855843</v>
       </c>
       <c r="J59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K59" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4490,10 +4490,10 @@
         <v>0.27959554760129218</v>
       </c>
       <c r="J60" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K60" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4526,10 +4526,10 @@
         <v>0.24640660988275187</v>
       </c>
       <c r="J61" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K61" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -4562,10 +4562,10 @@
         <v>0.31248687464999064</v>
       </c>
       <c r="J62" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K62" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -4598,10 +4598,10 @@
         <v>0.30219535020933891</v>
       </c>
       <c r="J63" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K63" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -4634,10 +4634,10 @@
         <v>0.38531777514067039</v>
       </c>
       <c r="J64" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K64" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -4670,10 +4670,10 @@
         <v>0.49322940132545562</v>
       </c>
       <c r="J65" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K65" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -4706,10 +4706,10 @@
         <v>0.17646334604027966</v>
       </c>
       <c r="J66" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K66" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -4742,10 +4742,10 @@
         <v>0.33030725263426475</v>
       </c>
       <c r="J67" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K67" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -4778,10 +4778,10 @@
         <v>0.19870810481331139</v>
       </c>
       <c r="J68" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K68" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -4814,10 +4814,10 @@
         <v>0.19591644695144098</v>
       </c>
       <c r="J69" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K69" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -4850,10 +4850,10 @@
         <v>0.10834686886247366</v>
       </c>
       <c r="J70" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K70" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -4886,10 +4886,10 @@
         <v>0.26880302338410939</v>
       </c>
       <c r="J71" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K71" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -4922,10 +4922,10 @@
         <v>0.22822555598866462</v>
       </c>
       <c r="J72" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K72" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -4958,10 +4958,10 @@
         <v>1</v>
       </c>
       <c r="J73" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K73" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -4994,10 +4994,10 @@
         <v>0.29703924607992427</v>
       </c>
       <c r="J74" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K74" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -5030,10 +5030,10 @@
         <v>0.70296075392007573</v>
       </c>
       <c r="J75" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K75" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -5066,10 +5066,10 @@
         <v>1</v>
       </c>
       <c r="J76" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K76" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -5102,10 +5102,10 @@
         <v>1</v>
       </c>
       <c r="J77" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K77" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -5138,10 +5138,10 @@
         <v>9.8683301508015339E-2</v>
       </c>
       <c r="J78" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K78" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -5174,10 +5174,10 @@
         <v>0.21125599486303379</v>
       </c>
       <c r="J79" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K79" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -5210,10 +5210,10 @@
         <v>0.47926312584528546</v>
       </c>
       <c r="J80" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K80" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -5246,10 +5246,10 @@
         <v>0.21079757778366542</v>
       </c>
       <c r="J81" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K81" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -5282,10 +5282,10 @@
         <v>9.4578630047296414E-2</v>
       </c>
       <c r="J82" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K82" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -5318,10 +5318,10 @@
         <v>0.13589328714773377</v>
       </c>
       <c r="J83" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K83" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -5354,10 +5354,10 @@
         <v>0.15079615307679198</v>
       </c>
       <c r="J84" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K84" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -5390,10 +5390,10 @@
         <v>0.16286970119173735</v>
       </c>
       <c r="J85" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K85" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -5426,10 +5426,10 @@
         <v>0.1490940403990495</v>
       </c>
       <c r="J86" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K86" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -5462,10 +5462,10 @@
         <v>0.20581820580090143</v>
       </c>
       <c r="J87" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K87" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -5498,10 +5498,10 @@
         <v>0.10094998233648955</v>
       </c>
       <c r="J88" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K88" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -5534,10 +5534,10 @@
         <v>0.95288203355075196</v>
       </c>
       <c r="J89" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K89" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -5570,10 +5570,10 @@
         <v>2.2922863306776509E-2</v>
       </c>
       <c r="J90" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K90" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -5606,10 +5606,10 @@
         <v>2.4195103142471565E-2</v>
       </c>
       <c r="J91" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K91" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -5642,10 +5642,10 @@
         <v>0.25257849202195715</v>
       </c>
       <c r="J92" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K92" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -5678,10 +5678,10 @@
         <v>0.29270570994389372</v>
       </c>
       <c r="J93" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K93" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -5714,10 +5714,10 @@
         <v>0.26929339914019479</v>
       </c>
       <c r="J94" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K94" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -5750,10 +5750,10 @@
         <v>0.18542239889395434</v>
       </c>
       <c r="J95" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K95" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -5786,10 +5786,10 @@
         <v>0.13416796959618271</v>
       </c>
       <c r="J96" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K96" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -5822,10 +5822,10 @@
         <v>0.33284458126227712</v>
       </c>
       <c r="J97" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K97" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -5858,10 +5858,10 @@
         <v>0.24054762090719262</v>
       </c>
       <c r="J98" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K98" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -5894,10 +5894,10 @@
         <v>0.29243982823434755</v>
       </c>
       <c r="J99" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K99" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -5930,10 +5930,10 @@
         <v>0.52333474415344183</v>
       </c>
       <c r="J100" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K100" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -5966,10 +5966,10 @@
         <v>0.47666525584655822</v>
       </c>
       <c r="J101" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K101" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -6002,10 +6002,10 @@
         <v>0.11483942067108532</v>
       </c>
       <c r="J102" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K102" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -6038,10 +6038,10 @@
         <v>0.29797143459108066</v>
       </c>
       <c r="J103" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K103" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -6074,10 +6074,10 @@
         <v>9.4665567759801159E-2</v>
       </c>
       <c r="J104" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K104" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -6110,10 +6110,10 @@
         <v>8.9296844417992405E-2</v>
       </c>
       <c r="J105" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K105" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -6146,10 +6146,10 @@
         <v>0.21429357679148961</v>
       </c>
       <c r="J106" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K106" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -6182,10 +6182,10 @@
         <v>0.14291050034957625</v>
       </c>
       <c r="J107" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K107" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -6218,10 +6218,10 @@
         <v>4.6022655418974601E-2</v>
       </c>
       <c r="J108" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K108" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -6254,10 +6254,10 @@
         <v>0.39952949924897041</v>
       </c>
       <c r="J109" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K109" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -6290,10 +6290,10 @@
         <v>0.43309725291582346</v>
       </c>
       <c r="J110" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K110" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -6326,10 +6326,10 @@
         <v>0.16737324783520613</v>
       </c>
       <c r="J111" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K111" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>